<commit_message>
MatBlazior : suite des tests
</commit_message>
<xml_diff>
--- a/Docs/Controles - Comparatif.xlsx
+++ b/Docs/Controles - Comparatif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tests\BlazorTests\BlazorTests\BlazorTests\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43603FA-8806-4778-819C-A66D39C44762}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC83AED-E062-4464-8757-2D639A162523}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10060D01-B858-415F-A4DA-C412A010DB92}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="49">
   <si>
     <t>Syncfusion</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>Value de type string
@@ -176,9 +179,6 @@
   <si>
     <t>Binding : KO (Impossible de retirer la valeur une fois mise)
 Mandatory : KO (même raison)</t>
-  </si>
-  <si>
-    <t>KO (System.InvalidOperationException: Cannot provide a value for property 'Http')</t>
   </si>
   <si>
     <r>
@@ -208,6 +208,18 @@
   <si>
     <t>Binding OK/KO (uniquement decimal? et pas int?)
 Champs obligatoires KO (fonctionne mais pas de trait sous le controle en cas d'erreur)</t>
+  </si>
+  <si>
+    <t>Mitigé : fonctionne très bien mais nécessite d'ajouter le code de boite de dialogue dans la page HTML</t>
+  </si>
+  <si>
+    <t>KO  : System.InvalidOperationException: Cannot provide a value for property 'Http'</t>
+  </si>
+  <si>
+    <t>Binding : KO (Value de type string uniquement + les données s'affichent mais je n'arrive pas à binder la valeur à ma propriété)</t>
+  </si>
+  <si>
+    <t>KO : Il existe un autocomplete mais je ne sais pas trop s'il sait gérer le chargement dynamique. Tous les exemples sont permettent uniquement de rechercher les valeurs en saisissant un texte.</t>
   </si>
 </sst>
 </file>
@@ -651,7 +663,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +745,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -759,7 +771,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -785,7 +797,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -811,7 +823,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -863,7 +875,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -967,7 +979,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J12" s="4"/>
     </row>
@@ -997,7 +1009,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1018,7 +1030,9 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1042,7 +1056,9 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="8"/>
+      <c r="I15" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1066,7 +1082,9 @@
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1090,10 +1108,12 @@
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="10"/>
+      <c r="I17" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1114,10 +1134,12 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="8"/>
+      <c r="I18" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1138,7 +1160,9 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Syncfusion : les onglets sont gérés correctement
</commit_message>
<xml_diff>
--- a/Docs/Controles - Comparatif.xlsx
+++ b/Docs/Controles - Comparatif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tests\BlazorTests\BlazorTests\BlazorTests\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DBCFB3-C620-4B38-A799-BAB115D9C59E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC0CF9E-08E0-4CF2-AE66-6A926CE4EE3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{10060D01-B858-415F-A4DA-C412A010DB92}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10060D01-B858-415F-A4DA-C412A010DB92}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="59">
   <si>
     <t>Syncfusion</t>
   </si>
@@ -281,9 +281,6 @@
       </rPr>
       <t>Mandatory : KO (pas possible de binder sur un champ non nullable)</t>
     </r>
-  </si>
-  <si>
-    <t>KO car ne gère pas la notion de Template</t>
   </si>
   <si>
     <t>Mitigé car fonctionne mais impossible d'afficher une date française et le filtrage ne fonctionne que si on saisit le texte complet</t>
@@ -475,11 +472,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852B876C-CFEA-4C71-98FB-34E755BFEB43}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,25 +806,25 @@
     <col min="4" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="48.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="1" customWidth="1"/>
     <col min="9" max="9" width="75.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -909,7 +906,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>51</v>
@@ -1118,8 +1115,8 @@
       <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>53</v>
+      <c r="G11" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>37</v>
@@ -1149,7 +1146,7 @@
         <v>28</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>37</v>
@@ -1179,10 +1176,10 @@
         <v>27</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>37</v>
@@ -1209,7 +1206,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>48</v>
@@ -1239,7 +1236,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>37</v>
@@ -1298,7 +1295,7 @@
       <c r="F17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H17" s="9" t="s">
@@ -1328,7 +1325,7 @@
       <c r="F18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H18" s="9" t="s">
@@ -1359,7 +1356,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>49</v>
@@ -1418,7 +1415,7 @@
       <c r="F21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H21" s="9" t="s">
@@ -1446,7 +1443,7 @@
       <c r="F22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H22" s="9" t="s">
@@ -1474,7 +1471,7 @@
       <c r="F23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H23" s="9" t="s">
@@ -1502,10 +1499,10 @@
       <c r="F24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>50</v>
       </c>
       <c r="I24" s="9"/>
@@ -1558,7 +1555,7 @@
       <c r="F26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H26" s="9" t="s">
@@ -1586,7 +1583,7 @@
       <c r="F27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H27" s="9" t="s">
@@ -1614,7 +1611,7 @@
       <c r="F28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H28" s="9" t="s">
@@ -1642,10 +1639,10 @@
       <c r="F29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>50</v>
       </c>
       <c r="I29" s="9"/>

</xml_diff>

<commit_message>
Syncfusion : possibilité de filtrer une grille à partir d'un contrôle Search global
</commit_message>
<xml_diff>
--- a/Docs/Controles - Comparatif.xlsx
+++ b/Docs/Controles - Comparatif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tests\BlazorTests\BlazorTests\BlazorTests\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC0CF9E-08E0-4CF2-AE66-6A926CE4EE3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55E7A9-AF4D-4FDE-A733-BE50C3A77262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10060D01-B858-415F-A4DA-C412A010DB92}"/>
   </bookViews>
@@ -281,9 +281,6 @@
       </rPr>
       <t>Mandatory : KO (pas possible de binder sur un champ non nullable)</t>
     </r>
-  </si>
-  <si>
-    <t>Mitigé car fonctionne mais impossible d'afficher une date française et le filtrage ne fonctionne que si on saisit le texte complet</t>
   </si>
   <si>
     <t>Mitigé car uniquement si défini par code</t>
@@ -333,6 +330,9 @@
   <si>
     <t>Binding : OK
 Mandatory : KO (je ne sais pas comment définir un élément vide)</t>
+  </si>
+  <si>
+    <t>Mitigé car fonctionne mais impossible d'afficher une date française</t>
   </si>
 </sst>
 </file>
@@ -795,7 +795,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>51</v>
@@ -1146,7 +1146,7 @@
         <v>28</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>37</v>
@@ -1176,10 +1176,10 @@
         <v>27</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>37</v>
@@ -1206,7 +1206,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>48</v>
@@ -1236,7 +1236,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>37</v>
@@ -1356,7 +1356,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Mise à jour fichier Excel comparatif
</commit_message>
<xml_diff>
--- a/Docs/Controles - Comparatif.xlsx
+++ b/Docs/Controles - Comparatif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tests\BlazorTests\BlazorTests\BlazorTests\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55E7A9-AF4D-4FDE-A733-BE50C3A77262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CD10EA-2C55-4EB0-8006-EB1B6BBEC691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10060D01-B858-415F-A4DA-C412A010DB92}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="57">
   <si>
     <t>Syncfusion</t>
   </si>
@@ -284,12 +284,6 @@
   </si>
   <si>
     <t>Mitigé car uniquement si défini par code</t>
-  </si>
-  <si>
-    <t>KO. Je n'arrive pas à le faire fonctionner</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> KO. Ne fonctionne pas</t>
   </si>
   <si>
     <r>
@@ -794,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852B876C-CFEA-4C71-98FB-34E755BFEB43}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +900,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>51</v>
@@ -1146,7 +1140,7 @@
         <v>28</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>37</v>
@@ -1205,8 +1199,8 @@
       <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>54</v>
+      <c r="G14" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>48</v>
@@ -1235,8 +1229,8 @@
       <c r="F15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>55</v>
+      <c r="G15" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>37</v>
@@ -1356,7 +1350,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>49</v>

</xml_diff>